<commit_message>
Update path collect for ZTE UME
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e13cb156cc9c7c4/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{4343332F-A6B2-4BC8-804D-5FCC4CE9960D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7F2A762-7852-40EF-A89A-181873530775}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054AD8CA-4E9B-434B-949D-5548F4F9DC59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backup!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Backup (2)'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="202">
   <si>
     <t>ZTE</t>
   </si>
@@ -804,6 +804,12 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RADIONODE_GSM/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/ZTE_UME/bulkcm/1Current/</t>
+  </si>
+  <si>
+    <t>ITBBU.xml</t>
   </si>
 </sst>
 </file>
@@ -1338,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4452,7 +4458,35 @@
         <v>52</v>
       </c>
     </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A108" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D108" s="23">
+        <v>2600</v>
+      </c>
+      <c r="E108" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F108" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G108" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="H108" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="I108" s="23"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{2A387F8D-CD5E-48AD-9A04-0BE6C4CE063A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update add 1800 Anchor, itbbu file 4G
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054AD8CA-4E9B-434B-949D-5548F4F9DC59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C8E7B-7740-4FD5-B817-48D765E61FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="202">
   <si>
     <t>ZTE</t>
   </si>
@@ -1344,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4484,6 +4484,33 @@
         <v>201</v>
       </c>
       <c r="I108" s="23"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A109" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D109" s="23">
+        <v>2600</v>
+      </c>
+      <c r="E109" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F109" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="H109" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="I109" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2A387F8D-CD5E-48AD-9A04-0BE6C4CE063A}"/>

</xml_diff>

<commit_message>
Update mapping Huawei 5G
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8360C6CE-4981-45DE-A252-0228BBF24C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4635F22-5239-4F47-B6BD-64DE04440163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="204">
   <si>
     <t>ZTE</t>
   </si>
@@ -810,6 +810,12 @@
   </si>
   <si>
     <t>.*UMEID_ITBBU_ZTE_.*.xml</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Huawei2100/BMA/CFGDATA/1Current</t>
+  </si>
+  <si>
+    <t>CFGDATA.XML</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4511,6 +4517,60 @@
         <v>201</v>
       </c>
       <c r="I109" s="23"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A110" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D110" s="23">
+        <v>2600</v>
+      </c>
+      <c r="E110" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F110" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G110" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="H110" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I110" s="23"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A111" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D111" s="23">
+        <v>2600</v>
+      </c>
+      <c r="E111" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F111" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="H111" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I111" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2A387F8D-CD5E-48AD-9A04-0BE6C4CE063A}"/>

</xml_diff>

<commit_message>
Update path for 5G huawei DEV
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4635F22-5239-4F47-B6BD-64DE04440163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59578241-E9BF-4DDD-91B0-22CE920C29CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -812,10 +812,10 @@
     <t>.*UMEID_ITBBU_ZTE_.*.xml</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Huawei2100/BMA/CFGDATA/1Current</t>
-  </si>
-  <si>
     <t>CFGDATA.XML</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Huawei2100/BMA/CFGDATA/1Current/</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4538,10 +4538,10 @@
         <v>13</v>
       </c>
       <c r="G110" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="H110" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="H110" s="25" t="s">
-        <v>203</v>
       </c>
       <c r="I110" s="23"/>
     </row>
@@ -4565,10 +4565,10 @@
         <v>13</v>
       </c>
       <c r="G111" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="H111" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="H111" s="25" t="s">
-        <v>203</v>
       </c>
       <c r="I111" s="23"/>
     </row>

</xml_diff>

<commit_message>
Update datasource for dev
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59578241-E9BF-4DDD-91B0-22CE920C29CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550B97A6-BDF2-433C-BB6B-EBBAC8592F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
+    <workbookView xWindow="60" yWindow="165" windowWidth="28740" windowHeight="15435" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
   <sheets>
     <sheet name="Path" sheetId="2" r:id="rId1"/>
@@ -815,7 +815,7 @@
     <t>CFGDATA.XML</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Huawei2100/BMA/CFGDATA/1Current/</t>
+    <t>/home/app/ngoss/data/rfserver/Huawei2600/BMA/CFGDATA/1Current/</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update huawei path configure and gzip file handle
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550B97A6-BDF2-433C-BB6B-EBBAC8592F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EB91A9-A7A0-4715-B92E-A1098B4DE0C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="165" windowWidth="28740" windowHeight="15435" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
   <sheets>
     <sheet name="Path" sheetId="2" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="207">
   <si>
     <t>ZTE</t>
   </si>
@@ -812,10 +812,19 @@
     <t>.*UMEID_ITBBU_ZTE_.*.xml</t>
   </si>
   <si>
-    <t>CFGDATA.XML</t>
-  </si>
-  <si>
-    <t>/home/app/ngoss/data/rfserver/Huawei2600/BMA/CFGDATA/1Current/</t>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_8/1Current/</t>
+  </si>
+  <si>
+    <t>CFGDATA_.*XML*</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE8/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_8/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_8/1Current/</t>
   </si>
 </sst>
 </file>
@@ -950,7 +959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1035,6 +1044,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4465,7 +4477,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A108" s="23" t="s">
+      <c r="A108" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B108" s="25" t="s">
@@ -4474,13 +4486,13 @@
       <c r="C108" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D108" s="23">
+      <c r="D108" s="33">
         <v>2600</v>
       </c>
-      <c r="E108" s="23" t="s">
+      <c r="E108" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F108" s="23" t="s">
+      <c r="F108" s="33" t="s">
         <v>13</v>
       </c>
       <c r="G108" s="25" t="s">
@@ -4489,10 +4501,10 @@
       <c r="H108" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="I108" s="23"/>
+      <c r="I108" s="33"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A109" s="23" t="s">
+      <c r="A109" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="25" t="s">
@@ -4501,13 +4513,13 @@
       <c r="C109" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D109" s="23">
+      <c r="D109" s="33">
         <v>2600</v>
       </c>
-      <c r="E109" s="23" t="s">
+      <c r="E109" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F109" s="23" t="s">
+      <c r="F109" s="33" t="s">
         <v>13</v>
       </c>
       <c r="G109" s="25" t="s">
@@ -4516,37 +4528,37 @@
       <c r="H109" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="I109" s="23"/>
+      <c r="I109" s="33"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A110" s="23" t="s">
+      <c r="A110" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C110" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="D110" s="23">
+        <v>16</v>
+      </c>
+      <c r="D110" s="33">
         <v>2600</v>
       </c>
-      <c r="E110" s="23" t="s">
+      <c r="E110" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F110" s="23" t="s">
+      <c r="F110" s="33" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="H110" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="H110" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="I110" s="23"/>
+      <c r="I110" s="33"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A111" s="23" t="s">
+      <c r="A111" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="25" t="s">
@@ -4555,22 +4567,184 @@
       <c r="C111" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D111" s="23">
+      <c r="D111" s="33">
         <v>2600</v>
       </c>
-      <c r="E111" s="23" t="s">
+      <c r="E111" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F111" s="23" t="s">
+      <c r="F111" s="33" t="s">
         <v>13</v>
       </c>
       <c r="G111" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="H111" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="H111" s="25" t="s">
+      <c r="I111" s="33"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A112" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D112" s="33">
+        <v>2600</v>
+      </c>
+      <c r="E112" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F112" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G112" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="H112" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I112" s="33"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A113" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113" s="33">
+        <v>2600</v>
+      </c>
+      <c r="E113" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F113" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G113" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="H113" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I113" s="33"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A114" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D114" s="33">
+        <v>2600</v>
+      </c>
+      <c r="E114" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F114" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G114" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="I111" s="23"/>
+      <c r="H114" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I114" s="33"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A115" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" s="33">
+        <v>2600</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F115" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G115" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="H115" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I115" s="33"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A116" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D116" s="33">
+        <v>2600</v>
+      </c>
+      <c r="E116" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F116" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="H116" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I116" s="33"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A117" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B117" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D117" s="33">
+        <v>2600</v>
+      </c>
+      <c r="E117" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F117" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G117" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="H117" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I117" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2A387F8D-CD5E-48AD-9A04-0BE6C4CE063A}"/>

</xml_diff>

<commit_message>
Fix path collector regex
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EB91A9-A7A0-4715-B92E-A1098B4DE0C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3DBB7-DF8B-4ECC-9F7A-5DDE1E777FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -815,9 +815,6 @@
     <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_8/1Current/</t>
   </si>
   <si>
-    <t>CFGDATA_.*XML*</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE8/1Current/</t>
   </si>
   <si>
@@ -825,6 +822,9 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_8/1Current/</t>
+  </si>
+  <si>
+    <t>CFGDATA_.*XML.*</t>
   </si>
 </sst>
 </file>
@@ -1042,11 +1042,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1365,7 +1365,7 @@
   <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G125" sqref="G125"/>
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4477,7 +4477,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A108" s="33" t="s">
+      <c r="A108" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B108" s="25" t="s">
@@ -4486,13 +4486,13 @@
       <c r="C108" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D108" s="33">
+      <c r="D108" s="32">
         <v>2600</v>
       </c>
-      <c r="E108" s="33" t="s">
+      <c r="E108" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F108" s="33" t="s">
+      <c r="F108" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G108" s="25" t="s">
@@ -4501,10 +4501,10 @@
       <c r="H108" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="I108" s="33"/>
+      <c r="I108" s="32"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A109" s="33" t="s">
+      <c r="A109" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="25" t="s">
@@ -4513,13 +4513,13 @@
       <c r="C109" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D109" s="33">
+      <c r="D109" s="32">
         <v>2600</v>
       </c>
-      <c r="E109" s="33" t="s">
+      <c r="E109" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F109" s="33" t="s">
+      <c r="F109" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G109" s="25" t="s">
@@ -4528,10 +4528,10 @@
       <c r="H109" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="I109" s="33"/>
+      <c r="I109" s="32"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A110" s="33" t="s">
+      <c r="A110" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="25" t="s">
@@ -4540,25 +4540,25 @@
       <c r="C110" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D110" s="33">
+      <c r="D110" s="32">
         <v>2600</v>
       </c>
-      <c r="E110" s="33" t="s">
+      <c r="E110" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F110" s="33" t="s">
+      <c r="F110" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="25" t="s">
         <v>202</v>
       </c>
       <c r="H110" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I110" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="I110" s="32"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A111" s="33" t="s">
+      <c r="A111" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="25" t="s">
@@ -4567,25 +4567,25 @@
       <c r="C111" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D111" s="33">
+      <c r="D111" s="32">
         <v>2600</v>
       </c>
-      <c r="E111" s="33" t="s">
+      <c r="E111" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F111" s="33" t="s">
+      <c r="F111" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G111" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H111" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I111" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="I111" s="32"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B112" s="25" t="s">
@@ -4594,25 +4594,25 @@
       <c r="C112" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D112" s="33">
+      <c r="D112" s="32">
         <v>2600</v>
       </c>
-      <c r="E112" s="33" t="s">
+      <c r="E112" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F112" s="33" t="s">
+      <c r="F112" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G112" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H112" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I112" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="I112" s="32"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A113" s="33" t="s">
+      <c r="A113" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B113" s="25" t="s">
@@ -4621,25 +4621,25 @@
       <c r="C113" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D113" s="33">
+      <c r="D113" s="32">
         <v>2600</v>
       </c>
-      <c r="E113" s="33" t="s">
+      <c r="E113" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F113" s="33" t="s">
+      <c r="F113" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G113" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="H113" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="H113" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I113" s="33"/>
+      <c r="I113" s="32"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A114" s="33" t="s">
+      <c r="A114" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B114" s="25" t="s">
@@ -4648,25 +4648,25 @@
       <c r="C114" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D114" s="33">
+      <c r="D114" s="32">
         <v>2600</v>
       </c>
-      <c r="E114" s="33" t="s">
+      <c r="E114" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F114" s="33" t="s">
+      <c r="F114" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G114" s="25" t="s">
         <v>202</v>
       </c>
       <c r="H114" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I114" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="I114" s="32"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A115" s="33" t="s">
+      <c r="A115" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B115" s="25" t="s">
@@ -4675,25 +4675,25 @@
       <c r="C115" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D115" s="33">
+      <c r="D115" s="32">
         <v>2600</v>
       </c>
-      <c r="E115" s="33" t="s">
+      <c r="E115" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F115" s="33" t="s">
+      <c r="F115" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H115" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I115" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="I115" s="32"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A116" s="33" t="s">
+      <c r="A116" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B116" s="25" t="s">
@@ -4702,25 +4702,25 @@
       <c r="C116" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D116" s="33">
+      <c r="D116" s="32">
         <v>2600</v>
       </c>
-      <c r="E116" s="33" t="s">
+      <c r="E116" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F116" s="33" t="s">
+      <c r="F116" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H116" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I116" s="33"/>
+        <v>206</v>
+      </c>
+      <c r="I116" s="32"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A117" s="33" t="s">
+      <c r="A117" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B117" s="25" t="s">
@@ -4729,22 +4729,22 @@
       <c r="C117" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D117" s="33">
+      <c r="D117" s="32">
         <v>2600</v>
       </c>
-      <c r="E117" s="33" t="s">
+      <c r="E117" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F117" s="33" t="s">
+      <c r="F117" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G117" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="H117" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="H117" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I117" s="33"/>
+      <c r="I117" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2A387F8D-CD5E-48AD-9A04-0BE6C4CE063A}"/>
@@ -7602,7 +7602,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -7613,7 +7613,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -7626,7 +7626,7 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="32"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7637,7 +7637,7 @@
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7648,7 +7648,7 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -7657,7 +7657,7 @@
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
@@ -7666,7 +7666,7 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="32"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="32"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
@@ -7689,7 +7689,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -7700,7 +7700,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -7713,7 +7713,7 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="32"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
@@ -7724,7 +7724,7 @@
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="1" t="s">
         <v>20</v>
       </c>
@@ -7737,7 +7737,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
@@ -7746,7 +7746,7 @@
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
@@ -7755,7 +7755,7 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="32"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -7766,7 +7766,7 @@
       <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
@@ -7775,7 +7775,7 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -7784,7 +7784,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="33" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -7795,7 +7795,7 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="32"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -7806,7 +7806,7 @@
       <c r="E11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
@@ -7819,7 +7819,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -7828,7 +7828,7 @@
       <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="1" t="s">
         <v>21</v>
       </c>
@@ -7837,7 +7837,7 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="32"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -7848,7 +7848,7 @@
       <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Fix regex 5g huawei
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3DBB7-DF8B-4ECC-9F7A-5DDE1E777FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5035731A-5DE2-4EA8-8E96-10DAA1DDD618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -824,7 +824,7 @@
     <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_8/1Current/</t>
   </si>
   <si>
-    <t>CFGDATA_.*XML.*</t>
+    <t>.*CFGDATA_.*XML.*</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,7 @@
   <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
add source path for huawei LTE/NR
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5035731A-5DE2-4EA8-8E96-10DAA1DDD618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D6181F-7874-4664-BF61-BB28CABE420A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="276">
   <si>
     <t>ZTE</t>
   </si>
@@ -825,13 +825,220 @@
   </si>
   <si>
     <t>.*CFGDATA_.*XML.*</t>
+  </si>
+  <si>
+    <t>L900/1800/2100/2600</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Huawei2100/TECH/BTS3900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Huawei2100/TECH/BTS3900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Huawei2100/TECH/BTS5900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_8/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE7/1Current/</t>
+  </si>
+  <si>
+    <t>TECH</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS5900_7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_4/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_5/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS5900_8/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_6/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_7/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_8/1Current/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,6 +1076,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1362,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="D214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H236" sqref="H236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1373,7 +1586,7 @@
     <col min="1" max="1" width="13.6640625" style="24" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" style="26" customWidth="1"/>
     <col min="3" max="3" width="15.46484375" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="18.86328125" style="24" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.6640625" style="24" customWidth="1"/>
     <col min="7" max="7" width="107.19921875" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46" style="26" bestFit="1" customWidth="1"/>
@@ -4646,19 +4859,19 @@
         <v>9</v>
       </c>
       <c r="C114" s="25" t="s">
-        <v>166</v>
+        <v>16</v>
       </c>
       <c r="D114" s="32">
         <v>2600</v>
       </c>
       <c r="E114" s="32" t="s">
-        <v>34</v>
+        <v>254</v>
       </c>
       <c r="F114" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G114" s="25" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="H114" s="25" t="s">
         <v>206</v>
@@ -4673,19 +4886,19 @@
         <v>9</v>
       </c>
       <c r="C115" s="25" t="s">
-        <v>166</v>
+        <v>16</v>
       </c>
       <c r="D115" s="32">
         <v>2600</v>
       </c>
       <c r="E115" s="32" t="s">
-        <v>34</v>
+        <v>254</v>
       </c>
       <c r="F115" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="H115" s="25" t="s">
         <v>206</v>
@@ -4700,19 +4913,19 @@
         <v>9</v>
       </c>
       <c r="C116" s="25" t="s">
-        <v>166</v>
+        <v>16</v>
       </c>
       <c r="D116" s="32">
         <v>2600</v>
       </c>
       <c r="E116" s="32" t="s">
-        <v>34</v>
+        <v>254</v>
       </c>
       <c r="F116" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="H116" s="25" t="s">
         <v>206</v>
@@ -4727,10 +4940,10 @@
         <v>9</v>
       </c>
       <c r="C117" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="D117" s="32">
-        <v>2600</v>
+        <v>16</v>
+      </c>
+      <c r="D117" s="23" t="s">
+        <v>207</v>
       </c>
       <c r="E117" s="32" t="s">
         <v>34</v>
@@ -4739,15 +4952,3634 @@
         <v>13</v>
       </c>
       <c r="G117" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="H117" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I117" s="32"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A118" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E118" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F118" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G118" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="H118" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I118" s="32"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A119" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E119" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F119" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G119" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="H119" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I119" s="32"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A120" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E120" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F120" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G120" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="H120" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I120" s="32"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A121" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B121" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D121" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E121" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F121" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G121" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="H121" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I121" s="32"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A122" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E122" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F122" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="H122" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I122" s="23"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A123" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E123" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F123" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G123" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H123" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I123" s="23"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A124" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B124" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E124" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F124" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G124" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="H124" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I124" s="23"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A125" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E125" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F125" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H125" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I125" s="23"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A126" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E126" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F126" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G126" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="H126" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I126" s="23"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A127" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E127" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F127" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="H127" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I127" s="23"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A128" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E128" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F128" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G128" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="H128" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I128" s="23"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A129" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E129" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F129" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G129" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="H129" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I129" s="23"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A130" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E130" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F130" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G130" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="H130" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I130" s="23"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A131" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E131" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F131" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G131" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H131" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I131" s="23"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A132" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D132" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E132" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F132" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G132" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="H132" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I132" s="23"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A133" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D133" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E133" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F133" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G133" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="H133" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I133" s="23"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A134" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D134" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E134" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F134" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G134" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="H134" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I134" s="23"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A135" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D135" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E135" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F135" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G135" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="H135" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I135" s="23"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A136" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D136" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E136" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F136" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G136" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="H136" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I136" s="23"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A137" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B137" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D137" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E137" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F137" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G137" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H137" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I137" s="23"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A138" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E138" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F138" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G138" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="H138" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I138" s="23"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A139" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B139" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D139" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E139" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F139" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G139" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="H139" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I139" s="23"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A140" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B140" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D140" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E140" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F140" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G140" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="H140" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I140" s="23"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A141" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B141" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C141" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D141" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E141" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F141" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G141" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="H141" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I141" s="23"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A142" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D142" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E142" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F142" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G142" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H142" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I142" s="23"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A143" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D143" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E143" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F143" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G143" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="H143" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I143" s="23"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A144" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D144" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E144" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F144" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G144" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="H144" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I144" s="23"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A145" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D145" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E145" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F145" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G145" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="H145" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I145" s="23"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A146" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D146" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E146" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F146" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G146" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="H146" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I146" s="23"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A147" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D147" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E147" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F147" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G147" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="H147" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I147" s="23"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A148" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D148" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E148" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F148" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G148" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="H148" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I148" s="23"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A149" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D149" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E149" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F149" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G149" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="H149" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I149" s="23"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A150" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D150" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E150" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F150" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G150" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="H150" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I150" s="23"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A151" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E151" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F151" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G151" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="H151" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I151" s="23"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A152" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D152" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E152" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F152" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G152" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="H152" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I152" s="23"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A153" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C153" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D153" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E153" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F153" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G153" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="H153" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I153" s="23"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A154" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B154" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C154" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D154" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E154" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F154" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G154" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="H154" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I154" s="23"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A155" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E155" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F155" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G155" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="H155" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I155" s="23"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A156" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B156" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D156" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E156" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F156" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="H156" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I156" s="23"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A157" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D157" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E157" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F157" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G157" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H157" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I157" s="23"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A158" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B158" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C158" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D158" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E158" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F158" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G158" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="H158" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I158" s="23"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A159" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B159" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C159" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D159" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E159" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F159" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G159" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="H159" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I159" s="23"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A160" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C160" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D160" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E160" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F160" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G160" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="H160" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I160" s="23"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A161" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D161" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E161" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F161" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G161" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="H161" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I161" s="23"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A162" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B162" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D162" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E162" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F162" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G162" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="H162" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I162" s="23"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A163" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B163" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C163" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D163" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E163" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F163" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G163" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="H163" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I163" s="23"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A164" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C164" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D164" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E164" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F164" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G164" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="H164" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I164" s="23"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A165" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C165" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D165" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E165" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F165" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G165" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="H165" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I165" s="23"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A166" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B166" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C166" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D166" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E166" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F166" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G166" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="H166" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I166" s="23"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A167" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B167" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D167" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E167" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F167" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G167" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="H167" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I167" s="23"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A168" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B168" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C168" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D168" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E168" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F168" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G168" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="H168" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I168" s="23"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A169" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B169" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C169" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D169" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E169" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F169" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G169" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="H169" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I169" s="23"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A170" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B170" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D170" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E170" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F170" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G170" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="H170" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I170" s="23"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A171" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B171" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C171" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D171" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E171" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F171" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G171" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="H171" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I171" s="23"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A172" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C172" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D172" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E172" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F172" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G172" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="H172" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I172" s="23"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A173" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C173" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D173" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E173" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F173" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G173" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="H173" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I173" s="23"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A174" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B174" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C174" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D174" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E174" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F174" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G174" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="H174" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I174" s="23"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A175" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D175" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E175" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F175" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G175" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="H175" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I175" s="23"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A176" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B176" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D176" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E176" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F176" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G176" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="H176" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I176" s="23"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A177" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B177" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D177" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E177" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F177" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G177" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="H177" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I177" s="23"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A178" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B178" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C178" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D178" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E178" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F178" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G178" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="H178" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I178" s="23"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A179" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B179" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C179" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D179" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E179" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F179" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G179" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="H179" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I179" s="23"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A180" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B180" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D180" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E180" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F180" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G180" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="H180" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I180" s="23"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A181" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B181" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D181" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E181" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F181" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G181" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="H181" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I181" s="32"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A182" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B182" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D182" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E182" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F182" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G182" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="H182" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I182" s="32"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A183" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B183" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C183" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D183" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E183" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F183" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G183" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="H183" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I183" s="32"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A184" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B184" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D184" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E184" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F184" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G184" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="H117" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="I117" s="32"/>
+      <c r="H184" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I184" s="32"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A185" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D185" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E185" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="F185" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G185" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="H185" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I185" s="32"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A186" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B186" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C186" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D186" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E186" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="F186" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G186" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="H186" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I186" s="32"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A187" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B187" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C187" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D187" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E187" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="F187" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G187" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="H187" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I187" s="32"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A188" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B188" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C188" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D188" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E188" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F188" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G188" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="H188" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I188" s="32"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A189" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B189" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C189" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D189" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E189" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F189" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G189" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="H189" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I189" s="32"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A190" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B190" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D190" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E190" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F190" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G190" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="H190" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I190" s="32"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A191" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B191" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C191" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D191" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E191" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F191" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G191" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="H191" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I191" s="32"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A192" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B192" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C192" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D192" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E192" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F192" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G192" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="H192" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I192" s="32"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A193" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B193" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D193" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E193" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F193" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G193" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="H193" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I193" s="23"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A194" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B194" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C194" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D194" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E194" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F194" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G194" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H194" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I194" s="23"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A195" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B195" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D195" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E195" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F195" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G195" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="H195" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I195" s="23"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A196" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B196" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C196" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D196" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E196" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F196" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G196" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H196" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I196" s="23"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A197" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B197" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C197" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D197" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E197" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F197" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G197" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="H197" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I197" s="23"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A198" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B198" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C198" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D198" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E198" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F198" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G198" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="H198" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I198" s="23"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A199" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B199" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C199" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D199" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E199" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F199" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G199" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="H199" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I199" s="23"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A200" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B200" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C200" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D200" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E200" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F200" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G200" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="H200" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I200" s="23"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A201" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B201" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C201" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D201" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E201" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F201" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G201" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="H201" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I201" s="23"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A202" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B202" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C202" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D202" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E202" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F202" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G202" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H202" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I202" s="23"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A203" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B203" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C203" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D203" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E203" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F203" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G203" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="H203" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I203" s="23"/>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A204" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B204" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C204" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D204" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E204" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F204" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G204" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="H204" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I204" s="23"/>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A205" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B205" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C205" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D205" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E205" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F205" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G205" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="H205" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I205" s="23"/>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A206" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B206" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C206" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D206" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E206" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F206" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G206" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="H206" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I206" s="23"/>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A207" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B207" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C207" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D207" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E207" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F207" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G207" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="H207" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I207" s="23"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A208" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B208" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C208" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D208" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E208" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F208" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G208" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H208" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I208" s="23"/>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A209" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C209" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D209" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E209" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F209" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G209" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="H209" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I209" s="23"/>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A210" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B210" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C210" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D210" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E210" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F210" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G210" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="H210" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I210" s="23"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A211" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C211" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D211" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E211" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F211" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G211" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="H211" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I211" s="23"/>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A212" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B212" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C212" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D212" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E212" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F212" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G212" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="H212" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I212" s="23"/>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A213" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B213" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C213" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D213" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E213" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F213" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G213" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H213" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I213" s="23"/>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A214" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B214" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C214" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D214" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E214" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F214" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G214" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="H214" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I214" s="23"/>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A215" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B215" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C215" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D215" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E215" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F215" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G215" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="H215" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I215" s="23"/>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A216" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B216" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D216" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E216" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F216" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G216" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="H216" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I216" s="23"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A217" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B217" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C217" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D217" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E217" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F217" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G217" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="H217" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I217" s="23"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A218" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B218" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C218" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D218" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E218" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F218" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G218" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="H218" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I218" s="23"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A219" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B219" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C219" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D219" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E219" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F219" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G219" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="H219" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I219" s="23"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A220" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B220" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D220" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E220" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F220" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G220" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="H220" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I220" s="23"/>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A221" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B221" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C221" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D221" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E221" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F221" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G221" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="H221" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I221" s="23"/>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A222" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B222" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C222" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D222" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E222" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F222" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G222" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="H222" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I222" s="23"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A223" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B223" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C223" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D223" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E223" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F223" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G223" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="H223" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I223" s="23"/>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A224" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B224" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C224" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D224" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E224" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F224" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G224" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="H224" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I224" s="23"/>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A225" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B225" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C225" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D225" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E225" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F225" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G225" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="H225" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I225" s="23"/>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A226" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B226" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C226" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D226" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E226" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F226" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G226" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="H226" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I226" s="23"/>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A227" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B227" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C227" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D227" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E227" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F227" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G227" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="H227" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I227" s="23"/>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A228" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B228" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C228" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D228" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E228" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F228" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G228" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H228" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I228" s="23"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A229" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B229" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C229" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D229" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E229" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F229" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G229" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="H229" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I229" s="23"/>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A230" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B230" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C230" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D230" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E230" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F230" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G230" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="H230" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I230" s="23"/>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A231" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B231" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C231" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D231" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E231" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F231" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G231" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="H231" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I231" s="23"/>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A232" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B232" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C232" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D232" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E232" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F232" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G232" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="H232" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I232" s="23"/>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A233" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B233" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C233" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D233" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E233" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F233" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G233" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="H233" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I233" s="23"/>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A234" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B234" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C234" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D234" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E234" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F234" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G234" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="H234" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I234" s="23"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A235" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B235" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C235" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D235" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E235" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F235" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G235" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="H235" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I235" s="23"/>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A236" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B236" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C236" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D236" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E236" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F236" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G236" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="H236" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I236" s="23"/>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A237" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B237" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C237" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D237" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E237" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F237" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G237" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="H237" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I237" s="23"/>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A238" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B238" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C238" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D238" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E238" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F238" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G238" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="H238" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I238" s="23"/>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A239" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B239" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D239" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E239" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F239" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G239" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="H239" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I239" s="23"/>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A240" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B240" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C240" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D240" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E240" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F240" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G240" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="H240" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I240" s="23"/>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A241" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B241" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C241" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D241" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E241" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F241" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G241" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="H241" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I241" s="23"/>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A242" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B242" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C242" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D242" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E242" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F242" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G242" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="H242" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I242" s="23"/>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A243" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B243" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C243" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D243" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E243" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F243" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G243" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="H243" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I243" s="23"/>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A244" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B244" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C244" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D244" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E244" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F244" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G244" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="H244" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I244" s="23"/>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A245" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B245" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C245" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D245" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E245" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F245" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G245" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="H245" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I245" s="23"/>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A246" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B246" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C246" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D246" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E246" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F246" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G246" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="H246" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I246" s="23"/>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A247" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B247" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C247" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D247" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E247" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F247" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G247" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="H247" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I247" s="23"/>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A248" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B248" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C248" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D248" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E248" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F248" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G248" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="H248" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I248" s="23"/>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A249" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B249" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C249" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D249" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E249" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F249" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G249" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="H249" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I249" s="23"/>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A250" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B250" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C250" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D250" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E250" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F250" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G250" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="H250" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I250" s="23"/>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A251" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B251" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C251" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D251" s="32">
+        <v>2600</v>
+      </c>
+      <c r="E251" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F251" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G251" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="H251" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="I251" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2A387F8D-CD5E-48AD-9A04-0BE6C4CE063A}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
update source for test
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A706F1CC-7FD6-4E6B-A617-592E01761486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D482EE-245D-4D8D-B307-B80486FAB2A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -812,9 +812,6 @@
     <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_8/1Current/</t>
   </si>
   <si>
-    <t>.*UMEID_ITBBU_ZTE_.*.xml</t>
-  </si>
-  <si>
     <t>.*CFGDATA_.*XML.*</t>
   </si>
   <si>
@@ -861,6 +858,9 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/EXERT/1Current/</t>
+  </si>
+  <si>
+    <t>.*_ITBBU_ZTE_.*.xml</t>
   </si>
 </sst>
 </file>
@@ -1396,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1462,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>49</v>
@@ -1491,7 +1491,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>60</v>
@@ -1810,7 +1810,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>39</v>
@@ -1839,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>39</v>
@@ -1868,7 +1868,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H16" s="24" t="s">
         <v>39</v>
@@ -1897,7 +1897,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H17" s="24" t="s">
         <v>39</v>
@@ -1926,7 +1926,7 @@
         <v>13</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>39</v>
@@ -1955,7 +1955,7 @@
         <v>13</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>39</v>
@@ -1984,7 +1984,7 @@
         <v>13</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H20" s="24" t="s">
         <v>39</v>
@@ -2013,7 +2013,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H21" s="24" t="s">
         <v>39</v>
@@ -2042,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H22" s="24" t="s">
         <v>39</v>
@@ -3661,7 +3661,7 @@
         <v>197</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="I78" s="29"/>
     </row>
@@ -3688,7 +3688,7 @@
         <v>197</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="I79" s="29"/>
     </row>
@@ -3715,7 +3715,7 @@
         <v>198</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I80" s="29"/>
     </row>
@@ -3742,7 +3742,7 @@
         <v>199</v>
       </c>
       <c r="H81" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I81" s="29"/>
     </row>
@@ -3769,7 +3769,7 @@
         <v>200</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I82" s="29"/>
     </row>
@@ -3796,7 +3796,7 @@
         <v>201</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I83" s="29"/>
     </row>
@@ -3811,7 +3811,7 @@
         <v>16</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E84" s="29" t="s">
         <v>58</v>
@@ -3820,10 +3820,10 @@
         <v>13</v>
       </c>
       <c r="G84" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H84" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I84" s="29"/>
     </row>
@@ -3838,7 +3838,7 @@
         <v>16</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E85" s="29" t="s">
         <v>58</v>
@@ -3847,10 +3847,10 @@
         <v>13</v>
       </c>
       <c r="G85" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H85" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I85" s="29"/>
     </row>
@@ -3865,7 +3865,7 @@
         <v>16</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E86" s="29" t="s">
         <v>58</v>
@@ -3874,10 +3874,10 @@
         <v>13</v>
       </c>
       <c r="G86" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H86" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I86" s="29"/>
     </row>
@@ -3904,7 +3904,7 @@
         <v>198</v>
       </c>
       <c r="H87" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I87" s="29"/>
     </row>
@@ -3931,7 +3931,7 @@
         <v>199</v>
       </c>
       <c r="H88" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I88" s="29"/>
     </row>
@@ -3958,7 +3958,7 @@
         <v>200</v>
       </c>
       <c r="H89" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I89" s="29"/>
     </row>
@@ -3985,7 +3985,7 @@
         <v>201</v>
       </c>
       <c r="H90" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I90" s="29"/>
     </row>
@@ -4009,10 +4009,10 @@
         <v>13</v>
       </c>
       <c r="G91" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H91" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I91" s="29"/>
     </row>
@@ -4036,10 +4036,10 @@
         <v>13</v>
       </c>
       <c r="G92" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H92" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I92" s="29"/>
     </row>
@@ -4063,10 +4063,10 @@
         <v>13</v>
       </c>
       <c r="G93" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H93" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I93" s="29"/>
     </row>

</xml_diff>

<commit_message>
Add region for parsing ericsson 4G
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D482EE-245D-4D8D-B307-B80486FAB2A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB11D237-735B-43FD-9ED7-C13E51BF7A8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backup!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Backup (2)'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="226">
   <si>
     <t>ZTE</t>
   </si>
@@ -692,9 +692,6 @@
     <t>xx_OMMR_xx12xx_umts_radio_xx.xml</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_LW/1Current</t>
-  </si>
-  <si>
     <t>NR</t>
   </si>
   <si>
@@ -710,18 +707,12 @@
     <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_LWG/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_LG/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/RNC/1Current/</t>
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/RBS/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/RADIONODE_WCDMA/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_WG/1Current/</t>
   </si>
   <si>
@@ -737,24 +728,15 @@
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RADIONODE/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_LW/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_LWG/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_LG/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RNC/1Current/</t>
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RBS/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RADIONODE_WCDMA/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_WG/1Current/</t>
   </si>
   <si>
@@ -770,24 +752,15 @@
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RADIONODE/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_LW/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_LWG/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_LG/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RNC/1Current/</t>
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RBS/1Current/</t>
   </si>
   <si>
-    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RADIONODE_WCDMA/1Current</t>
-  </si>
-  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_WG/1Current/</t>
   </si>
   <si>
@@ -812,6 +785,9 @@
     <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/NodeB3900_8/1Current/</t>
   </si>
   <si>
+    <t>.*UMEID_ITBBU_ZTE_.*.xml</t>
+  </si>
+  <si>
     <t>.*CFGDATA_.*XML.*</t>
   </si>
   <si>
@@ -860,14 +836,59 @@
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/EXERT/1Current/</t>
   </si>
   <si>
-    <t>.*_ITBBU_ZTE_.*.xml</t>
+    <t>700/2600</t>
+  </si>
+  <si>
+    <t>700/2601</t>
+  </si>
+  <si>
+    <t>700/2602</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/CNA_FULL/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/EXERT/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/CNA_FULL/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/EXERT/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/RADIONODE_WCDMA/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_LW/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_LW/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RADIONODE_WCDMA/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_LW/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RADIONODE_WCDMA/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_NL/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_NL/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_NL/1Current/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,6 +926,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1394,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1462,7 +1489,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>49</v>
@@ -1491,7 +1518,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>60</v>
@@ -1520,7 +1547,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>83</v>
+        <v>213</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>49</v>
@@ -1549,7 +1576,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>84</v>
+        <v>214</v>
       </c>
       <c r="H5" s="24" t="s">
         <v>56</v>
@@ -1578,7 +1605,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>49</v>
@@ -1607,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="H7" s="24" t="s">
         <v>56</v>
@@ -1624,7 +1651,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" s="29">
         <v>2600</v>
@@ -1636,7 +1663,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H8" s="24" t="s">
         <v>51</v>
@@ -1653,7 +1680,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D9" s="29">
         <v>2600</v>
@@ -1665,7 +1692,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>51</v>
@@ -1682,7 +1709,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" s="29">
         <v>2600</v>
@@ -1694,7 +1721,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H10" s="24" t="s">
         <v>51</v>
@@ -1810,7 +1837,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>39</v>
@@ -1839,7 +1866,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>39</v>
@@ -1868,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H16" s="24" t="s">
         <v>39</v>
@@ -1897,7 +1924,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H17" s="24" t="s">
         <v>39</v>
@@ -1926,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>39</v>
@@ -1955,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>39</v>
@@ -1984,7 +2011,7 @@
         <v>13</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H20" s="24" t="s">
         <v>39</v>
@@ -2013,7 +2040,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H21" s="24" t="s">
         <v>39</v>
@@ -2042,7 +2069,7 @@
         <v>13</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H22" s="24" t="s">
         <v>39</v>
@@ -2411,7 +2438,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>51</v>
@@ -2440,7 +2467,7 @@
         <v>13</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H36" s="24" t="s">
         <v>51</v>
@@ -2469,7 +2496,7 @@
         <v>13</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>51</v>
@@ -2498,7 +2525,7 @@
         <v>13</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H38" s="24" t="s">
         <v>51</v>
@@ -2527,7 +2554,7 @@
         <v>13</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H39" s="24" t="s">
         <v>51</v>
@@ -2556,7 +2583,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="H40" s="24" t="s">
         <v>51</v>
@@ -2585,7 +2612,7 @@
         <v>13</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H41" s="24" t="s">
         <v>51</v>
@@ -2614,7 +2641,7 @@
         <v>13</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="H42" s="24" t="s">
         <v>51</v>
@@ -2643,7 +2670,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H43" s="24" t="s">
         <v>51</v>
@@ -2672,7 +2699,7 @@
         <v>13</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H44" s="24" t="s">
         <v>51</v>
@@ -2701,7 +2728,7 @@
         <v>13</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H45" s="24" t="s">
         <v>51</v>
@@ -2730,7 +2757,7 @@
         <v>13</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H46" s="24" t="s">
         <v>51</v>
@@ -2759,7 +2786,7 @@
         <v>13</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H47" s="24" t="s">
         <v>51</v>
@@ -2788,7 +2815,7 @@
         <v>13</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H48" s="24" t="s">
         <v>51</v>
@@ -2817,7 +2844,7 @@
         <v>13</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H49" s="24" t="s">
         <v>51</v>
@@ -2846,7 +2873,7 @@
         <v>13</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="H50" s="24" t="s">
         <v>51</v>
@@ -2875,7 +2902,7 @@
         <v>13</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H51" s="24" t="s">
         <v>51</v>
@@ -2904,7 +2931,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H52" s="24" t="s">
         <v>51</v>
@@ -2933,7 +2960,7 @@
         <v>13</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H53" s="24" t="s">
         <v>51</v>
@@ -2962,7 +2989,7 @@
         <v>13</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>51</v>
@@ -2991,7 +3018,7 @@
         <v>13</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="H55" s="24" t="s">
         <v>51</v>
@@ -3020,7 +3047,7 @@
         <v>13</v>
       </c>
       <c r="G56" s="24" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H56" s="24" t="s">
         <v>51</v>
@@ -3049,7 +3076,7 @@
         <v>13</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="H57" s="24" t="s">
         <v>51</v>
@@ -3078,7 +3105,7 @@
         <v>13</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H58" s="24" t="s">
         <v>51</v>
@@ -3107,7 +3134,7 @@
         <v>13</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H59" s="24" t="s">
         <v>51</v>
@@ -3136,7 +3163,7 @@
         <v>13</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H60" s="24" t="s">
         <v>51</v>
@@ -3165,7 +3192,7 @@
         <v>13</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="H61" s="24" t="s">
         <v>51</v>
@@ -3194,7 +3221,7 @@
         <v>13</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H62" s="24" t="s">
         <v>51</v>
@@ -3223,7 +3250,7 @@
         <v>13</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H63" s="24" t="s">
         <v>51</v>
@@ -3252,7 +3279,7 @@
         <v>13</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H64" s="24" t="s">
         <v>51</v>
@@ -3281,7 +3308,7 @@
         <v>13</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="H65" s="24" t="s">
         <v>51</v>
@@ -3310,7 +3337,7 @@
         <v>13</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H66" s="24" t="s">
         <v>51</v>
@@ -3339,7 +3366,7 @@
         <v>13</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H67" s="24" t="s">
         <v>51</v>
@@ -3368,7 +3395,7 @@
         <v>13</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H68" s="24" t="s">
         <v>51</v>
@@ -3397,7 +3424,7 @@
         <v>13</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H69" s="24" t="s">
         <v>51</v>
@@ -3426,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="H70" s="24" t="s">
         <v>51</v>
@@ -3455,7 +3482,7 @@
         <v>13</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H71" s="24" t="s">
         <v>51</v>
@@ -3484,7 +3511,7 @@
         <v>13</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="H72" s="24" t="s">
         <v>51</v>
@@ -3513,7 +3540,7 @@
         <v>13</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H73" s="24" t="s">
         <v>51</v>
@@ -3542,7 +3569,7 @@
         <v>13</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="H74" s="24" t="s">
         <v>51</v>
@@ -3571,7 +3598,7 @@
         <v>13</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H75" s="24" t="s">
         <v>51</v>
@@ -3600,7 +3627,7 @@
         <v>13</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H76" s="24" t="s">
         <v>51</v>
@@ -3629,7 +3656,7 @@
         <v>13</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H77" s="24" t="s">
         <v>51</v>
@@ -3646,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D78" s="29">
         <v>2600</v>
@@ -3658,10 +3685,10 @@
         <v>13</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="I78" s="29"/>
     </row>
@@ -3685,10 +3712,10 @@
         <v>13</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="I79" s="29"/>
     </row>
@@ -3712,10 +3739,10 @@
         <v>13</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I80" s="29"/>
     </row>
@@ -3739,10 +3766,10 @@
         <v>13</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H81" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I81" s="29"/>
     </row>
@@ -3766,10 +3793,10 @@
         <v>13</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I82" s="29"/>
     </row>
@@ -3793,10 +3820,10 @@
         <v>13</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I83" s="29"/>
     </row>
@@ -3811,7 +3838,7 @@
         <v>16</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E84" s="29" t="s">
         <v>58</v>
@@ -3820,10 +3847,10 @@
         <v>13</v>
       </c>
       <c r="G84" s="24" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H84" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I84" s="29"/>
     </row>
@@ -3838,7 +3865,7 @@
         <v>16</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E85" s="29" t="s">
         <v>58</v>
@@ -3847,10 +3874,10 @@
         <v>13</v>
       </c>
       <c r="G85" s="24" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H85" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I85" s="29"/>
     </row>
@@ -3865,7 +3892,7 @@
         <v>16</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E86" s="29" t="s">
         <v>58</v>
@@ -3874,10 +3901,10 @@
         <v>13</v>
       </c>
       <c r="G86" s="24" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H86" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I86" s="29"/>
     </row>
@@ -3889,7 +3916,7 @@
         <v>9</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D87" s="29">
         <v>2600</v>
@@ -3901,10 +3928,10 @@
         <v>13</v>
       </c>
       <c r="G87" s="24" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H87" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I87" s="29"/>
     </row>
@@ -3916,7 +3943,7 @@
         <v>9</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D88" s="29">
         <v>2600</v>
@@ -3928,10 +3955,10 @@
         <v>13</v>
       </c>
       <c r="G88" s="24" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H88" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I88" s="29"/>
     </row>
@@ -3943,7 +3970,7 @@
         <v>9</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D89" s="29">
         <v>2600</v>
@@ -3955,10 +3982,10 @@
         <v>13</v>
       </c>
       <c r="G89" s="24" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H89" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I89" s="29"/>
     </row>
@@ -3970,7 +3997,7 @@
         <v>9</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D90" s="29">
         <v>2600</v>
@@ -3982,10 +4009,10 @@
         <v>13</v>
       </c>
       <c r="G90" s="24" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="H90" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I90" s="29"/>
     </row>
@@ -3997,7 +4024,7 @@
         <v>9</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D91" s="29">
         <v>2600</v>
@@ -4009,10 +4036,10 @@
         <v>13</v>
       </c>
       <c r="G91" s="24" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H91" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I91" s="29"/>
     </row>
@@ -4024,7 +4051,7 @@
         <v>9</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D92" s="29">
         <v>2600</v>
@@ -4036,10 +4063,10 @@
         <v>13</v>
       </c>
       <c r="G92" s="24" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H92" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I92" s="29"/>
     </row>
@@ -4051,7 +4078,7 @@
         <v>9</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D93" s="29">
         <v>2600</v>
@@ -4063,15 +4090,190 @@
         <v>13</v>
       </c>
       <c r="G93" s="24" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H93" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I93" s="29"/>
     </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A94" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="H94" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I94" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A95" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E95" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="H95" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I95" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A96" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F96" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H96" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I96" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A97" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F97" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="H97" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I97" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A98" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="H98" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I98" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A99" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E99" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F99" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H99" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I99" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I93" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
+  <autoFilter ref="A1:I99" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
update excel for dev
</commit_message>
<xml_diff>
--- a/config/dev/RawFilePathCollection.xlsx
+++ b/config/dev/RawFilePathCollection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\git\true\ranbaseline\source\config\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFA4676-2A55-450C-B6B1-AB222CDF36FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75996C1-4AC1-4A75-AEC6-58E229F4A130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backup!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Backup (2)'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="227">
   <si>
     <t>ZTE</t>
   </si>
@@ -722,6 +722,12 @@
     <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/RADIONODE_GSM/1Current/</t>
   </si>
   <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/ENB/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RADIONODE/1Current/</t>
+  </si>
+  <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_LWG/1Current/</t>
   </si>
   <si>
@@ -738,6 +744,12 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RADIONODE_GSM/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/ENB/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RADIONODE/1Current/</t>
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_LWG/1Current/</t>
@@ -1412,10 +1424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1480,7 +1492,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>49</v>
@@ -1509,7 +1521,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>60</v>
@@ -1538,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>49</v>
@@ -1567,7 +1579,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H5" s="24" t="s">
         <v>56</v>
@@ -1596,7 +1608,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>49</v>
@@ -1625,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H7" s="24" t="s">
         <v>56</v>
@@ -1828,7 +1840,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>39</v>
@@ -1857,7 +1869,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>39</v>
@@ -1886,7 +1898,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H16" s="24" t="s">
         <v>39</v>
@@ -1915,7 +1927,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="H17" s="24" t="s">
         <v>39</v>
@@ -1944,7 +1956,7 @@
         <v>13</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>39</v>
@@ -1973,7 +1985,7 @@
         <v>13</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>39</v>
@@ -2002,7 +2014,7 @@
         <v>13</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H20" s="24" t="s">
         <v>39</v>
@@ -2031,7 +2043,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="H21" s="24" t="s">
         <v>39</v>
@@ -2060,7 +2072,7 @@
         <v>13</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H22" s="24" t="s">
         <v>39</v>
@@ -2359,10 +2371,10 @@
         <v>17</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D33" s="29">
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>55</v>
@@ -2371,7 +2383,7 @@
         <v>13</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="H33" s="24" t="s">
         <v>51</v>
@@ -2388,10 +2400,10 @@
         <v>17</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>55</v>
@@ -2400,7 +2412,7 @@
         <v>13</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="H34" s="24" t="s">
         <v>51</v>
@@ -2417,10 +2429,10 @@
         <v>17</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>55</v>
@@ -2429,7 +2441,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>51</v>
@@ -2446,10 +2458,10 @@
         <v>17</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>55</v>
@@ -2458,7 +2470,7 @@
         <v>13</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H36" s="24" t="s">
         <v>51</v>
@@ -2475,10 +2487,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>55</v>
@@ -2487,7 +2499,7 @@
         <v>13</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>51</v>
@@ -2516,7 +2528,7 @@
         <v>13</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H38" s="24" t="s">
         <v>51</v>
@@ -2533,10 +2545,10 @@
         <v>17</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D39" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E39" s="29" t="s">
         <v>55</v>
@@ -2545,13 +2557,13 @@
         <v>13</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H39" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I39" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
@@ -2562,10 +2574,10 @@
         <v>17</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D40" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>55</v>
@@ -2574,13 +2586,13 @@
         <v>13</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="H40" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I40" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -2591,10 +2603,10 @@
         <v>17</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D41" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E41" s="29" t="s">
         <v>55</v>
@@ -2603,13 +2615,13 @@
         <v>13</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H41" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I41" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2620,10 +2632,10 @@
         <v>17</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D42" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E42" s="29" t="s">
         <v>55</v>
@@ -2632,13 +2644,13 @@
         <v>13</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="H42" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I42" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -2655,13 +2667,13 @@
         <v>2100</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F43" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H43" s="24" t="s">
         <v>51</v>
@@ -2678,25 +2690,25 @@
         <v>17</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D44" s="29">
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F44" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H44" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -2707,25 +2719,25 @@
         <v>17</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D45" s="29">
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
       <c r="H45" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2736,25 +2748,25 @@
         <v>17</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D46" s="29">
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H46" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -2765,25 +2777,25 @@
         <v>17</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D47" s="29">
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F47" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="H47" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -2794,10 +2806,10 @@
         <v>17</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D48" s="29">
-        <v>2100</v>
+        <v>900</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>46</v>
@@ -2823,10 +2835,10 @@
         <v>17</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="29">
-        <v>900</v>
+        <v>16</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>46</v>
@@ -2835,13 +2847,13 @@
         <v>13</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H49" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I49" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
@@ -2852,10 +2864,10 @@
         <v>17</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="29">
-        <v>900</v>
+        <v>16</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>46</v>
@@ -2864,13 +2876,13 @@
         <v>13</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="H50" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I50" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
@@ -2881,10 +2893,10 @@
         <v>17</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="29">
-        <v>900</v>
+        <v>16</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>46</v>
@@ -2893,13 +2905,13 @@
         <v>13</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H51" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
@@ -2910,10 +2922,10 @@
         <v>17</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="29">
-        <v>900</v>
+        <v>16</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E52" s="29" t="s">
         <v>46</v>
@@ -2922,13 +2934,13 @@
         <v>13</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H52" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I52" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
@@ -2945,13 +2957,13 @@
         <v>2100</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F53" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H53" s="24" t="s">
         <v>51</v>
@@ -2974,13 +2986,13 @@
         <v>2100</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F54" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>51</v>
@@ -3003,13 +3015,13 @@
         <v>2100</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F55" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H55" s="24" t="s">
         <v>51</v>
@@ -3032,13 +3044,13 @@
         <v>2100</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F56" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G56" s="24" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H56" s="24" t="s">
         <v>51</v>
@@ -3061,13 +3073,13 @@
         <v>2100</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F57" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H57" s="24" t="s">
         <v>51</v>
@@ -3090,13 +3102,13 @@
         <v>2100</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F58" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H58" s="24" t="s">
         <v>51</v>
@@ -3119,13 +3131,13 @@
         <v>900</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F59" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H59" s="24" t="s">
         <v>51</v>
@@ -3148,13 +3160,13 @@
         <v>900</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F60" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H60" s="24" t="s">
         <v>51</v>
@@ -3177,13 +3189,13 @@
         <v>900</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F61" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H61" s="24" t="s">
         <v>51</v>
@@ -3206,13 +3218,13 @@
         <v>900</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H62" s="24" t="s">
         <v>51</v>
@@ -3221,614 +3233,1049 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>206</v>
+        <v>16</v>
+      </c>
+      <c r="D63" s="29">
+        <v>900</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F63" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H63" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="I63" s="29"/>
-    </row>
-    <row r="64" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+      <c r="I63" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C64" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>222</v>
+        <v>54</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F64" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H64" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="I64" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I64" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="29">
-        <v>2600</v>
+      <c r="D65" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F65" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I65" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I65" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D66" s="29">
-        <v>2600</v>
+      <c r="D66" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F66" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I66" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I66" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C67" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="29">
-        <v>2600</v>
+      <c r="D67" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F67" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H67" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I67" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I67" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D68" s="29">
-        <v>2600</v>
+        <v>2100</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F68" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I68" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I68" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D69" s="29" t="s">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="D69" s="29">
+        <v>2100</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F69" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H69" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I69" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I69" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="29" t="s">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="D70" s="29">
+        <v>2100</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F70" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I70" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I70" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D71" s="29" t="s">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="D71" s="29">
+        <v>2100</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F71" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I71" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I71" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D72" s="29">
-        <v>2600</v>
+        <v>2100</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F72" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I72" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I72" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D73" s="29">
-        <v>2600</v>
+        <v>2100</v>
       </c>
       <c r="E73" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F73" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H73" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I73" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I73" s="29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="D74" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F74" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I74" s="29"/>
-    </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+      <c r="I74" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="D75" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F75" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I75" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="D76" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F76" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I76" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I76" s="29" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="D77" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F77" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I77" s="29"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+      <c r="I77" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D78" s="29">
-        <v>2600</v>
+      <c r="D78" s="29" t="s">
+        <v>210</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F78" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I78" s="29"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A79" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>54</v>
+        <v>226</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F79" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I79" s="29" t="s">
-        <v>53</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="I79" s="29"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="29" t="s">
-        <v>54</v>
+      <c r="D80" s="29">
+        <v>2600</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F80" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I80" s="29" t="s">
-        <v>52</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I80" s="29"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D81" s="29" t="s">
-        <v>54</v>
+      <c r="D81" s="29">
+        <v>2600</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F81" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="H81" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I81" s="29" t="s">
-        <v>52</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I81" s="29"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D82" s="29" t="s">
-        <v>206</v>
+        <v>16</v>
+      </c>
+      <c r="D82" s="29">
+        <v>2600</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="F82" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I82" s="29" t="s">
-        <v>53</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I82" s="29"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D83" s="29" t="s">
-        <v>207</v>
+        <v>16</v>
+      </c>
+      <c r="D83" s="29">
+        <v>2600</v>
       </c>
       <c r="E83" s="29" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F83" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I83" s="29" t="s">
-        <v>52</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I83" s="29"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C84" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E84" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F84" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="H84" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I84" s="29"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A85" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E85" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G85" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H85" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I85" s="29"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A86" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F86" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="H86" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I86" s="29"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A87" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D84" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="E84" s="29" t="s">
+      <c r="D87" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F87" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="H87" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I87" s="29"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A88" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D88" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F88" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G88" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="H88" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I88" s="29"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A89" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D89" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E89" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F89" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="H89" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I89" s="29"/>
+    </row>
+    <row r="90" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D90" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F90" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H90" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I90" s="29"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A91" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D91" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F91" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="H91" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I91" s="29"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A92" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D92" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F92" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H92" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I92" s="29"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A93" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D93" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E93" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F93" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G93" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="H93" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I93" s="29"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A94" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="H94" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I94" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A95" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E95" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="H95" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I95" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A96" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E96" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F84" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="H84" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I84" s="29" t="s">
+      <c r="F96" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H96" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I96" s="29" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A97" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F97" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="H97" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I97" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A98" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="H98" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I98" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A99" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E99" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F99" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H99" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I99" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I84" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
+  <autoFilter ref="A1:I99" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>